<commit_message>
using anthrpic sonnet as its better
</commit_message>
<xml_diff>
--- a/uploaded_files/cleaned_Budget.xlsx
+++ b/uploaded_files/cleaned_Budget.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,421 +493,429 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Outsourced Items Rental</t>
+          <t xml:space="preserve"> Euphoria Décor</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>26611506</v>
+        <v>12726000</v>
       </c>
       <c r="C2" t="n">
-        <v>56000000</v>
+        <v>55000000</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>-29388494</v>
+        <v>-42274000</v>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>3.8</v>
       </c>
       <c r="I2" t="n">
-        <v>11.5</v>
+        <v>11.3</v>
       </c>
       <c r="J2" t="n">
-        <v>-52.5</v>
+        <v>-76.90000000000001</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.4</v>
+        <v>-7.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Euphoria Outsourced Items Rental</t>
+          <t xml:space="preserve"> Additional Food &amp; Stations</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12856000</v>
+        <v>5313320.3</v>
       </c>
       <c r="C3" t="n">
-        <v>22000000.36</v>
+        <v>3614401</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
-        <v>-9144000.359999999</v>
+        <v>1698919.3</v>
       </c>
       <c r="H3" t="n">
-        <v>3.9</v>
+        <v>1.6</v>
       </c>
       <c r="I3" t="n">
-        <v>4.5</v>
+        <v>0.7</v>
       </c>
       <c r="J3" t="n">
-        <v>-41.6</v>
+        <v>47</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.6</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Professional Services</t>
+          <t>Total Income</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4869650</v>
+        <v>331353937.29</v>
       </c>
       <c r="C4" t="n">
-        <v>6910000</v>
+        <v>488054751</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Expenses</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>Key KPI</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Subtotals</t>
+        </is>
+      </c>
       <c r="G4" t="n">
-        <v>-2040350</v>
+        <v>-156700813.71</v>
       </c>
       <c r="H4" t="n">
-        <v>1.5</v>
+        <v>100</v>
       </c>
       <c r="I4" t="n">
-        <v>1.4</v>
+        <v>100</v>
       </c>
       <c r="J4" t="n">
-        <v>-29.5</v>
+        <v>-32.1</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fuel Charges</t>
+          <t xml:space="preserve"> Other Dry Stock</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4097112</v>
+        <v>15404163</v>
       </c>
       <c r="C5" t="n">
-        <v>3650000</v>
+        <v>14766946</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Cost of Sales</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>447112</v>
+        <v>637217</v>
       </c>
       <c r="H5" t="n">
-        <v>1.2</v>
+        <v>4.6</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7</v>
+        <v>3</v>
       </c>
       <c r="J5" t="n">
-        <v>12.2</v>
+        <v>4.3</v>
       </c>
       <c r="K5" t="n">
-        <v>0.5</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Sales Rep Commission</t>
+          <t xml:space="preserve"> Dairy &amp; Bakery Items</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3301917</v>
+        <v>15684897</v>
       </c>
       <c r="C6" t="n">
-        <v>8153957</v>
+        <v>15563716</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Cost of Sales</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>-4852040</v>
+        <v>121181</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>4.7</v>
       </c>
       <c r="I6" t="n">
-        <v>1.7</v>
+        <v>3.2</v>
       </c>
       <c r="J6" t="n">
-        <v>-59.5</v>
+        <v>0.8</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fee &amp; Subcription</t>
+          <t xml:space="preserve"> Beverages &amp; Soft drinks</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3207958.47</v>
+        <v>5032509</v>
       </c>
       <c r="C7" t="n">
-        <v>4260000</v>
+        <v>13011841</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Cost of Sales</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>-1052041.53</v>
+        <v>-7979332</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9</v>
+        <v>2.7</v>
       </c>
       <c r="J7" t="n">
-        <v>-24.7</v>
+        <v>-61.3</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1</v>
+        <v>-1.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Office Rent</t>
+          <t xml:space="preserve"> Other Consumables</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2800700</v>
+        <v>7011284.6</v>
       </c>
       <c r="C8" t="n">
-        <v>3732000</v>
+        <v>5096683</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Cost of Sales</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
-        <v>-931300</v>
+        <v>1914601.6</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8</v>
+        <v>2.1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>-25</v>
+        <v>37.6</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Other benefits (Direct &amp; indrect)</t>
+          <t xml:space="preserve"> Wages &amp; Allowance</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2674364.25</v>
+        <v>7320065</v>
       </c>
       <c r="C9" t="n">
-        <v>2100000</v>
+        <v>13365667</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Cost of Sales</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>574364.25</v>
+        <v>-6045602</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8</v>
+        <v>2.2</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4</v>
+        <v>2.7</v>
       </c>
       <c r="J9" t="n">
-        <v>27.4</v>
+        <v>-45.2</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ad Spend</t>
+          <t xml:space="preserve"> Utilitites</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2174662.52</v>
+        <v>17459405.79</v>
       </c>
       <c r="C10" t="n">
-        <v>1925000</v>
+        <v>16942755</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Cost of Sales</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>249662.52</v>
+        <v>516650.7899999991</v>
       </c>
       <c r="H10" t="n">
-        <v>0.7</v>
+        <v>5.3</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4</v>
+        <v>3.5</v>
       </c>
       <c r="J10" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="K10" t="n">
-        <v>0.3</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Elecricity Charges</t>
+          <t>Total Cost of Sales</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1598528</v>
+        <v>257732956.39</v>
       </c>
       <c r="C11" t="n">
-        <v>3051096</v>
+        <v>326260705</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Expenses</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>Key KPI</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Subtotals</t>
+        </is>
+      </c>
       <c r="G11" t="n">
-        <v>-1452568</v>
+        <v>-68527748.61000001</v>
       </c>
       <c r="H11" t="n">
-        <v>0.5</v>
+        <v>77.8</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6</v>
+        <v>66.8</v>
       </c>
       <c r="J11" t="n">
-        <v>-47.6</v>
+        <v>-21</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.1</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Agency Fee</t>
+          <t>Gross Profit</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1320000</v>
+        <v>73620980.89999998</v>
       </c>
       <c r="C12" t="n">
-        <v>1800000</v>
+        <v>161794046</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Key KPI</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>-480000</v>
+        <v>-88173065.10000002</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4</v>
+        <v>22.2</v>
       </c>
       <c r="I12" t="n">
-        <v>0.4</v>
+        <v>33.2</v>
       </c>
       <c r="J12" t="n">
-        <v>-26.7</v>
+        <v>-54.5</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>-10.9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mobile Charges</t>
+          <t xml:space="preserve"> Marketing</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>747479.21</v>
+        <v>403667</v>
       </c>
       <c r="C13" t="n">
-        <v>542000</v>
+        <v>3240000</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -919,35 +927,35 @@
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>205479.21</v>
+        <v>-2836333</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="J13" t="n">
-        <v>37.9</v>
+        <v>-87.5</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Vehicles Repair</t>
+          <t xml:space="preserve"> Other benefits (Direct &amp; indrect)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>522224</v>
+        <v>2674364.25</v>
       </c>
       <c r="C14" t="n">
-        <v>704196.95</v>
+        <v>2100000</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -956,32 +964,32 @@
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>-181972.95</v>
+        <v>574364.25</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="J14" t="n">
-        <v>-25.8</v>
+        <v>27.4</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Office Supplies</t>
+          <t xml:space="preserve"> Toll Tax</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>469305</v>
+        <v>7110</v>
       </c>
       <c r="C15" t="n">
-        <v>360000</v>
+        <v>36000</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -993,32 +1001,32 @@
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>109305</v>
+        <v>-28890</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>30.4</v>
+        <v>-80.2</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Marketing</t>
+          <t xml:space="preserve"> Water Charges</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>403667</v>
+        <v>52020</v>
       </c>
       <c r="C16" t="n">
-        <v>3240000</v>
+        <v>339012</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1030,32 +1038,32 @@
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
-        <v>-2836333</v>
+        <v>-286992</v>
       </c>
       <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.1</v>
       </c>
-      <c r="I16" t="n">
-        <v>0.7</v>
-      </c>
       <c r="J16" t="n">
-        <v>-87.5</v>
+        <v>-84.7</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Stationary Expense</t>
+          <t xml:space="preserve"> Mobile Charges</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>359483</v>
+        <v>747479.21</v>
       </c>
       <c r="C17" t="n">
-        <v>300000</v>
+        <v>542000</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -1067,35 +1075,35 @@
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>59483</v>
+        <v>205479.21</v>
       </c>
       <c r="H17" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I17" t="n">
         <v>0.1</v>
       </c>
       <c r="J17" t="n">
-        <v>19.8</v>
+        <v>37.9</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Filing Fee</t>
+          <t xml:space="preserve"> Fuel Charges</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>288000</v>
+        <v>4097112</v>
       </c>
       <c r="C18" t="n">
-        <v>780000</v>
+        <v>3650000</v>
       </c>
       <c r="D18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1104,32 +1112,32 @@
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
-        <v>-492000</v>
+        <v>447112</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1</v>
+        <v>1.2</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="J18" t="n">
-        <v>-63.1</v>
+        <v>12.2</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bank Service Charges</t>
+          <t xml:space="preserve"> Local Traveling</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>284725.23</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>200319</v>
+        <v>165000</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -1141,35 +1149,35 @@
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
-        <v>84406.22999999998</v>
+        <v>-165000</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>42.1</v>
+        <v>-100</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Office Repair</t>
+          <t xml:space="preserve"> Office Supplies</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>273454</v>
+        <v>469305</v>
       </c>
       <c r="C20" t="n">
-        <v>454838.21</v>
+        <v>360000</v>
       </c>
       <c r="D20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1178,7 +1186,7 @@
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
-        <v>-181384.21</v>
+        <v>109305</v>
       </c>
       <c r="H20" t="n">
         <v>0.1</v>
@@ -1187,26 +1195,26 @@
         <v>0.1</v>
       </c>
       <c r="J20" t="n">
-        <v>-39.9</v>
+        <v>30.4</v>
       </c>
       <c r="K20" t="n">
-        <v>-0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Equipment Repair</t>
+          <t xml:space="preserve"> Stationary Expense</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>257905</v>
+        <v>359483</v>
       </c>
       <c r="C21" t="n">
-        <v>490004.84</v>
+        <v>300000</v>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1215,7 +1223,7 @@
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>-232099.84</v>
+        <v>59483</v>
       </c>
       <c r="H21" t="n">
         <v>0.1</v>
@@ -1224,23 +1232,23 @@
         <v>0.1</v>
       </c>
       <c r="J21" t="n">
-        <v>-47.4</v>
+        <v>19.8</v>
       </c>
       <c r="K21" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Toll Tax</t>
+          <t xml:space="preserve"> Ad Spend</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>7110</v>
+        <v>2174662.52</v>
       </c>
       <c r="C22" t="n">
-        <v>36000</v>
+        <v>1925000</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -1252,32 +1260,32 @@
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>-28890</v>
+        <v>249662.52</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J22" t="n">
-        <v>-80.2</v>
+        <v>13</v>
       </c>
       <c r="K22" t="n">
-        <v>-0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Water Charges</t>
+          <t xml:space="preserve"> Ad Production</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>52020</v>
+        <v>40000</v>
       </c>
       <c r="C23" t="n">
-        <v>339012</v>
+        <v>820000</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -1289,69 +1297,73 @@
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>-286992</v>
+        <v>-780000</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="J23" t="n">
-        <v>-84.7</v>
+        <v>-95.09999999999999</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Local Traveling</t>
+          <t>Total Expenses</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>30103402.84</v>
       </c>
       <c r="C24" t="n">
-        <v>165000</v>
+        <v>70728705</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Expenses</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
+          <t>Key KPI</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Subtotals</t>
+        </is>
+      </c>
       <c r="G24" t="n">
-        <v>-165000</v>
+        <v>-40625302.16</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="J24" t="n">
-        <v>-100</v>
+        <v>-57.4</v>
       </c>
       <c r="K24" t="n">
-        <v>-0</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ad Production</t>
+          <t xml:space="preserve"> Bank Service Charges</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>40000</v>
+        <v>284725.23</v>
       </c>
       <c r="C25" t="n">
-        <v>820000</v>
+        <v>200319</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -1363,19 +1375,19 @@
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
-        <v>-780000</v>
+        <v>84406.22999999998</v>
       </c>
       <c r="H25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I25" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="n">
-        <v>0.2</v>
-      </c>
       <c r="J25" t="n">
-        <v>-95.09999999999999</v>
+        <v>42.1</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1413,6 +1425,43 @@
       </c>
       <c r="K26" t="n">
         <v>-1.1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Net Income</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>68020707.32999997</v>
+      </c>
+      <c r="C27" t="n">
+        <v>78593112.64</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Key KPI</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>-10572405.31000003</v>
+      </c>
+      <c r="H27" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="I27" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-13.5</v>
+      </c>
+      <c r="K27" t="n">
+        <v>4.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>